<commit_message>
Included other team tests
</commit_message>
<xml_diff>
--- a/etc/2231-swen-261-07-j toasters.xlsx
+++ b/etc/2231-swen-261-07-j toasters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shade\Documents\SWEN-261\toasters\team-project-toasters\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theem\Documents\CodingProjects\team-project-toasters\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D93E37-FF20-4913-9107-74B9499D91B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFF1B75-AF6E-4425-B585-AA15ACE85B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="74">
   <si>
     <t>Instructions</t>
   </si>
@@ -653,6 +653,36 @@
   </si>
   <si>
     <t>Given that I enter an existing username when I select the "sign up" button, then I expect to see an error telling me that the user already exists</t>
+  </si>
+  <si>
+    <t>team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>There is no message - team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>we could not add the need to the funding basket from the main needs page, only once you click on the need do you see this option - team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>you have a typo in this acceptance criteria - team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>btw the need is removed from the cupboard when it is put into the cart, not just when you check out - team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>search does not work. There is no button to search the text that was typed. -team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>we like that it goes back to the cupboard once you do this - team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>this is fun! - team 1A 11/13/23</t>
+  </si>
+  <si>
+    <t>EH; 11/13/2023</t>
   </si>
 </sst>
 </file>
@@ -809,7 +839,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1230,9 +1294,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F587"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1279,7 +1343,12 @@
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
@@ -1292,7 +1361,12 @@
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -1305,7 +1379,12 @@
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1318,7 +1397,12 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
@@ -1331,7 +1415,12 @@
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1346,7 +1435,12 @@
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -1358,7 +1452,12 @@
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
@@ -1371,7 +1470,12 @@
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1386,7 +1490,12 @@
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -1398,7 +1507,12 @@
       <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
@@ -1411,7 +1525,12 @@
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1426,7 +1545,12 @@
       <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
@@ -1439,7 +1563,12 @@
       <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1454,7 +1583,12 @@
       <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
@@ -1467,9 +1601,14 @@
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>32</v>
       </c>
@@ -1482,9 +1621,14 @@
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -1497,9 +1641,14 @@
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="13" t="s">
         <v>35</v>
@@ -1510,9 +1659,14 @@
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -1525,9 +1679,14 @@
       <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1537,9 +1696,14 @@
       <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="13" t="s">
         <v>38</v>
@@ -1550,9 +1714,14 @@
       <c r="D22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>52</v>
       </c>
@@ -1565,9 +1734,14 @@
       <c r="D23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>53</v>
       </c>
@@ -1575,9 +1749,14 @@
         <v>41</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="E24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>42</v>
       </c>
@@ -1585,24 +1764,39 @@
         <v>43</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="E25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>54</v>
       </c>
@@ -1610,9 +1804,14 @@
         <v>46</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="E28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>55</v>
       </c>
@@ -1620,17 +1819,27 @@
         <v>56</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13" t="s">
         <v>57</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="E30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>58</v>
       </c>
@@ -1638,17 +1847,27 @@
         <v>59</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C32" s="8"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="E32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>61</v>
       </c>
@@ -1656,69 +1875,79 @@
         <v>62</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C39" s="8"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C40" s="8"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C42" s="8"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C43" s="8"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C46" s="8"/>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
     </row>
@@ -3880,20 +4109,36 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C587 E2:E587">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+  <conditionalFormatting sqref="C2:C587 E35:E587">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F587 D2:D587">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D587 F35:F587">
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E34">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F34">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(ISBLANK(F2),E2="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>AND(ISBLANK(F2),E2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>